<commit_message>
Changed some Alien Names
</commit_message>
<xml_diff>
--- a/sets/carddata.xlsx
+++ b/sets/carddata.xlsx
@@ -156,9 +156,6 @@
     <t>Soldier of Zarxxig</t>
   </si>
   <si>
-    <t>Alien Conquerer of the Thousand Universes, Yxxilizyzygzx</t>
-  </si>
-  <si>
     <t>Medieval</t>
   </si>
   <si>
@@ -514,6 +511,9 @@
   </si>
   <si>
     <t>Xylzig, Wanderer of Space</t>
+  </si>
+  <si>
+    <t>Uugvak, Conquerer of the Universe</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -892,24 +892,24 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -917,50 +917,50 @@
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -968,33 +968,33 @@
         <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,33 +1002,33 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1036,16 +1036,16 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,16 +1053,16 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,16 +1070,16 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1090,13 +1090,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,13 +1107,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,16 +1121,16 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1138,16 +1138,16 @@
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1155,16 +1155,16 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1172,16 +1172,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,13 +1192,13 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1209,13 +1209,13 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1226,13 +1226,13 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1243,30 +1243,30 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1277,13 +1277,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1294,13 +1294,13 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1311,13 +1311,13 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1328,30 +1328,30 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1362,13 +1362,13 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1376,50 +1376,50 @@
         <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
         <v>61</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" t="s">
         <v>62</v>
       </c>
-      <c r="C32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" t="s">
-        <v>63</v>
-      </c>
       <c r="E32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1430,30 +1430,30 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1464,13 +1464,13 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1478,16 +1478,16 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1495,16 +1495,16 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,16 +1512,16 @@
         <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1532,13 +1532,13 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1546,16 +1546,16 @@
         <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1563,16 +1563,16 @@
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1580,50 +1580,50 @@
         <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1631,16 +1631,16 @@
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1648,16 +1648,16 @@
         <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1665,16 +1665,16 @@
         <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1685,30 +1685,30 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1716,16 +1716,16 @@
         <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1736,353 +1736,353 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" t="s">
         <v>120</v>
       </c>
-      <c r="B53" t="s">
-        <v>121</v>
-      </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D55" t="s">
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
       </c>
       <c r="E56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
       </c>
       <c r="E57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" t="s">
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
         <v>126</v>
       </c>
-      <c r="B58" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" t="s">
-        <v>127</v>
-      </c>
       <c r="D58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>132</v>
+      </c>
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
         <v>133</v>
       </c>
-      <c r="B59" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59" t="s">
-        <v>134</v>
-      </c>
       <c r="D59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>134</v>
+      </c>
+      <c r="B60" t="s">
+        <v>120</v>
+      </c>
+      <c r="C60" t="s">
         <v>135</v>
       </c>
-      <c r="B60" t="s">
-        <v>121</v>
-      </c>
-      <c r="C60" t="s">
-        <v>136</v>
-      </c>
       <c r="D60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" t="s">
+        <v>120</v>
+      </c>
+      <c r="C61" t="s">
         <v>138</v>
       </c>
-      <c r="B61" t="s">
-        <v>121</v>
-      </c>
-      <c r="C61" t="s">
-        <v>139</v>
-      </c>
       <c r="D61" t="s">
         <v>5</v>
       </c>
       <c r="E61" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" t="s">
         <v>140</v>
       </c>
-      <c r="B62" t="s">
-        <v>121</v>
-      </c>
-      <c r="C62" t="s">
-        <v>141</v>
-      </c>
       <c r="D62" t="s">
         <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" t="s">
         <v>142</v>
       </c>
-      <c r="B63" t="s">
-        <v>121</v>
-      </c>
-      <c r="C63" t="s">
-        <v>143</v>
-      </c>
       <c r="D63" t="s">
         <v>5</v>
       </c>
       <c r="E63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" t="s">
+        <v>120</v>
+      </c>
+      <c r="C64" t="s">
         <v>144</v>
       </c>
-      <c r="B64" t="s">
-        <v>121</v>
-      </c>
-      <c r="C64" t="s">
-        <v>145</v>
-      </c>
       <c r="D64" t="s">
         <v>5</v>
       </c>
       <c r="E64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>145</v>
+      </c>
+      <c r="B65" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" t="s">
         <v>146</v>
       </c>
-      <c r="B65" t="s">
-        <v>121</v>
-      </c>
-      <c r="C65" t="s">
-        <v>147</v>
-      </c>
       <c r="D65" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E65" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>147</v>
+      </c>
+      <c r="B66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" t="s">
         <v>148</v>
       </c>
-      <c r="B66" t="s">
-        <v>121</v>
-      </c>
-      <c r="C66" t="s">
-        <v>149</v>
-      </c>
       <c r="D66" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" t="s">
+        <v>120</v>
+      </c>
+      <c r="C67" t="s">
         <v>150</v>
       </c>
-      <c r="B67" t="s">
-        <v>121</v>
-      </c>
-      <c r="C67" t="s">
-        <v>151</v>
-      </c>
       <c r="D67" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B68" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" t="s">
         <v>152</v>
       </c>
-      <c r="B68" t="s">
-        <v>121</v>
-      </c>
-      <c r="C68" t="s">
-        <v>153</v>
-      </c>
       <c r="D68" t="s">
         <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" t="s">
         <v>154</v>
       </c>
-      <c r="B69" t="s">
-        <v>121</v>
-      </c>
-      <c r="C69" t="s">
-        <v>155</v>
-      </c>
       <c r="D69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E69" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" t="s">
+        <v>120</v>
+      </c>
+      <c r="C70" t="s">
         <v>156</v>
       </c>
-      <c r="B70" t="s">
-        <v>121</v>
-      </c>
-      <c r="C70" t="s">
-        <v>157</v>
-      </c>
       <c r="D70" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E70" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>157</v>
+      </c>
+      <c r="B71" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" t="s">
         <v>158</v>
       </c>
-      <c r="B71" t="s">
-        <v>121</v>
-      </c>
-      <c r="C71" t="s">
-        <v>159</v>
-      </c>
       <c r="D71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E71" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed name of Alien Spawn
</commit_message>
<xml_diff>
--- a/sets/carddata.xlsx
+++ b/sets/carddata.xlsx
@@ -201,9 +201,6 @@
     <t>Rare</t>
   </si>
   <si>
-    <t>Alien Spawn</t>
-  </si>
-  <si>
     <t>Alien of Light, Oman</t>
   </si>
   <si>
@@ -514,6 +511,9 @@
   </si>
   <si>
     <t>Uugvak, Conquerer of the Universe</t>
+  </si>
+  <si>
+    <t>Kozex, Changeling</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -867,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -897,13 +897,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>
@@ -920,7 +920,7 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -937,7 +937,7 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -948,13 +948,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -971,7 +971,7 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -982,13 +982,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1005,7 +1005,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1016,13 +1016,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1039,7 +1039,7 @@
         <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1056,7 +1056,7 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -1073,7 +1073,7 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
@@ -1090,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -1107,7 +1107,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1124,7 +1124,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1141,7 +1141,7 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -1158,7 +1158,7 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D17" t="s">
         <v>49</v>
@@ -1175,7 +1175,7 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
@@ -1192,7 +1192,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1209,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
@@ -1226,7 +1226,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -1243,7 +1243,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
         <v>49</v>
@@ -1254,13 +1254,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -1277,7 +1277,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -1294,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
         <v>48</v>
@@ -1311,7 +1311,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
         <v>48</v>
@@ -1328,7 +1328,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
         <v>48</v>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -1362,7 +1362,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -1379,7 +1379,7 @@
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -1390,13 +1390,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
@@ -1407,16 +1407,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" t="s">
         <v>61</v>
-      </c>
-      <c r="C32" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" t="s">
-        <v>62</v>
       </c>
       <c r="E32" t="s">
         <v>54</v>
@@ -1430,7 +1430,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
         <v>48</v>
@@ -1441,13 +1441,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
@@ -1464,7 +1464,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -1481,7 +1481,7 @@
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
@@ -1498,7 +1498,7 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
         <v>48</v>
@@ -1515,7 +1515,7 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
         <v>48</v>
@@ -1532,7 +1532,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -1549,7 +1549,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
@@ -1566,7 +1566,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D41" t="s">
         <v>49</v>
@@ -1583,7 +1583,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" t="s">
         <v>48</v>
@@ -1594,13 +1594,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D43" t="s">
         <v>48</v>
@@ -1611,13 +1611,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1634,7 +1634,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
@@ -1651,7 +1651,7 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
@@ -1668,7 +1668,7 @@
         <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D47" t="s">
         <v>48</v>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D48" t="s">
         <v>48</v>
@@ -1702,7 +1702,7 @@
         <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
@@ -1719,7 +1719,7 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
@@ -1736,7 +1736,7 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -1753,7 +1753,7 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
@@ -1764,13 +1764,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
         <v>119</v>
       </c>
-      <c r="B53" t="s">
-        <v>120</v>
-      </c>
       <c r="C53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
@@ -1781,13 +1781,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D55" t="s">
         <v>5</v>
@@ -1815,13 +1815,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -1832,13 +1832,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
@@ -1849,16 +1849,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" t="s">
         <v>125</v>
       </c>
-      <c r="B58" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" t="s">
-        <v>126</v>
-      </c>
       <c r="D58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E58" t="s">
         <v>55</v>
@@ -1866,13 +1866,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" t="s">
         <v>132</v>
-      </c>
-      <c r="B59" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" t="s">
-        <v>133</v>
       </c>
       <c r="D59" t="s">
         <v>48</v>
@@ -1883,13 +1883,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s">
         <v>134</v>
-      </c>
-      <c r="B60" t="s">
-        <v>120</v>
-      </c>
-      <c r="C60" t="s">
-        <v>135</v>
       </c>
       <c r="D60" t="s">
         <v>48</v>
@@ -1900,13 +1900,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
         <v>137</v>
-      </c>
-      <c r="B61" t="s">
-        <v>120</v>
-      </c>
-      <c r="C61" t="s">
-        <v>138</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -1917,13 +1917,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
         <v>139</v>
-      </c>
-      <c r="B62" t="s">
-        <v>120</v>
-      </c>
-      <c r="C62" t="s">
-        <v>140</v>
       </c>
       <c r="D62" t="s">
         <v>5</v>
@@ -1934,13 +1934,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" t="s">
         <v>141</v>
-      </c>
-      <c r="B63" t="s">
-        <v>120</v>
-      </c>
-      <c r="C63" t="s">
-        <v>142</v>
       </c>
       <c r="D63" t="s">
         <v>5</v>
@@ -1951,13 +1951,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" t="s">
         <v>143</v>
-      </c>
-      <c r="B64" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" t="s">
-        <v>144</v>
       </c>
       <c r="D64" t="s">
         <v>5</v>
@@ -1968,13 +1968,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>144</v>
+      </c>
+      <c r="B65" t="s">
+        <v>119</v>
+      </c>
+      <c r="C65" t="s">
         <v>145</v>
-      </c>
-      <c r="B65" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" t="s">
-        <v>146</v>
       </c>
       <c r="D65" t="s">
         <v>48</v>
@@ -1985,13 +1985,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>146</v>
+      </c>
+      <c r="B66" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" t="s">
         <v>147</v>
-      </c>
-      <c r="B66" t="s">
-        <v>120</v>
-      </c>
-      <c r="C66" t="s">
-        <v>148</v>
       </c>
       <c r="D66" t="s">
         <v>48</v>
@@ -2002,13 +2002,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>148</v>
+      </c>
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" t="s">
         <v>149</v>
-      </c>
-      <c r="B67" t="s">
-        <v>120</v>
-      </c>
-      <c r="C67" t="s">
-        <v>150</v>
       </c>
       <c r="D67" t="s">
         <v>48</v>
@@ -2019,13 +2019,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>150</v>
+      </c>
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" t="s">
         <v>151</v>
-      </c>
-      <c r="B68" t="s">
-        <v>120</v>
-      </c>
-      <c r="C68" t="s">
-        <v>152</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
@@ -2036,13 +2036,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" t="s">
         <v>153</v>
-      </c>
-      <c r="B69" t="s">
-        <v>120</v>
-      </c>
-      <c r="C69" t="s">
-        <v>154</v>
       </c>
       <c r="D69" t="s">
         <v>49</v>
@@ -2053,13 +2053,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" t="s">
         <v>155</v>
-      </c>
-      <c r="B70" t="s">
-        <v>120</v>
-      </c>
-      <c r="C70" t="s">
-        <v>156</v>
       </c>
       <c r="D70" t="s">
         <v>48</v>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>156</v>
+      </c>
+      <c r="B71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" t="s">
         <v>157</v>
       </c>
-      <c r="B71" t="s">
-        <v>120</v>
-      </c>
-      <c r="C71" t="s">
-        <v>158</v>
-      </c>
       <c r="D71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E71" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Added A Few Generic Cards
</commit_message>
<xml_diff>
--- a/sets/carddata.xlsx
+++ b/sets/carddata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="168">
   <si>
     <t>Name</t>
   </si>
@@ -514,6 +514,24 @@
   </si>
   <si>
     <t>Kozex, Changeling</t>
+  </si>
+  <si>
+    <t>S220</t>
+  </si>
+  <si>
+    <t>Look Into the Future</t>
+  </si>
+  <si>
+    <t>S221</t>
+  </si>
+  <si>
+    <t>Ice Mammoth</t>
+  </si>
+  <si>
+    <t>S222</t>
+  </si>
+  <si>
+    <t>Necromancy</t>
   </si>
 </sst>
 </file>
@@ -857,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -865,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,6 +2103,57 @@
         <v>55</v>
       </c>
     </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>163</v>
+      </c>
+      <c r="B72" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" t="s">
+        <v>162</v>
+      </c>
+      <c r="D72" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>165</v>
+      </c>
+      <c r="B73" t="s">
+        <v>60</v>
+      </c>
+      <c r="C73" t="s">
+        <v>164</v>
+      </c>
+      <c r="D73" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>167</v>
+      </c>
+      <c r="B74" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" t="s">
+        <v>166</v>
+      </c>
+      <c r="D74" t="s">
+        <v>48</v>
+      </c>
+      <c r="E74" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:E51">
     <sortCondition ref="A2:A51"/>

</xml_diff>

<commit_message>
Changed Greater and Lesser Minion to Proper Name
</commit_message>
<xml_diff>
--- a/sets/carddata.xlsx
+++ b/sets/carddata.xlsx
@@ -219,15 +219,9 @@
     <t>Kingdom</t>
   </si>
   <si>
-    <t>Lesser Minion</t>
-  </si>
-  <si>
     <t>Alien Battlefield</t>
   </si>
   <si>
-    <t>Greater Minion</t>
-  </si>
-  <si>
     <t>S101</t>
   </si>
   <si>
@@ -532,6 +526,12 @@
   </si>
   <si>
     <t>Necromancy</t>
+  </si>
+  <si>
+    <t>Tundra Fox</t>
+  </si>
+  <si>
+    <t>Flying Snake</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -885,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,13 +915,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>
@@ -938,7 +938,7 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -955,7 +955,7 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -966,13 +966,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -989,7 +989,7 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -1006,7 +1006,7 @@
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -1023,7 +1023,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -1034,13 +1034,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1057,7 +1057,7 @@
         <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -1074,7 +1074,7 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
@@ -1091,7 +1091,7 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
@@ -1108,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -1125,7 +1125,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1142,7 +1142,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
@@ -1159,7 +1159,7 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -1176,7 +1176,7 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
         <v>49</v>
@@ -1193,7 +1193,7 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
@@ -1210,7 +1210,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
@@ -1227,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
         <v>50</v>
@@ -1244,7 +1244,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
         <v>48</v>
@@ -1261,7 +1261,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
         <v>49</v>
@@ -1272,13 +1272,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -1295,7 +1295,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -1312,7 +1312,7 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
         <v>48</v>
@@ -1329,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
         <v>48</v>
@@ -1346,7 +1346,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
         <v>48</v>
@@ -1357,13 +1357,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>167</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -1380,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -1397,7 +1397,7 @@
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -1408,13 +1408,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
@@ -1431,7 +1431,7 @@
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
         <v>61</v>
@@ -1448,7 +1448,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D33" t="s">
         <v>48</v>
@@ -1465,7 +1465,7 @@
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
@@ -1482,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
@@ -1499,7 +1499,7 @@
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
@@ -1516,7 +1516,7 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D37" t="s">
         <v>48</v>
@@ -1533,7 +1533,7 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
         <v>48</v>
@@ -1550,7 +1550,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
@@ -1567,7 +1567,7 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
@@ -1584,7 +1584,7 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D41" t="s">
         <v>49</v>
@@ -1601,7 +1601,7 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
         <v>48</v>
@@ -1612,13 +1612,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
         <v>48</v>
@@ -1629,13 +1629,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
@@ -1652,7 +1652,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
@@ -1669,7 +1669,7 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
@@ -1686,7 +1686,7 @@
         <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
         <v>48</v>
@@ -1703,7 +1703,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D48" t="s">
         <v>48</v>
@@ -1720,7 +1720,7 @@
         <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
@@ -1737,7 +1737,7 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
@@ -1754,7 +1754,7 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
@@ -1771,7 +1771,7 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
@@ -1782,13 +1782,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
@@ -1799,13 +1799,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
@@ -1816,13 +1816,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D55" t="s">
         <v>5</v>
@@ -1833,13 +1833,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -1850,13 +1850,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C57" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
@@ -1867,16 +1867,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D58" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E58" t="s">
         <v>55</v>
@@ -1884,13 +1884,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C59" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D59" t="s">
         <v>48</v>
@@ -1901,13 +1901,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D60" t="s">
         <v>48</v>
@@ -1918,13 +1918,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C61" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -1935,13 +1935,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D62" t="s">
         <v>5</v>
@@ -1952,13 +1952,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C63" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D63" t="s">
         <v>5</v>
@@ -1969,13 +1969,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D64" t="s">
         <v>48</v>
@@ -1986,13 +1986,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D65" t="s">
         <v>48</v>
@@ -2003,13 +2003,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D66" t="s">
         <v>48</v>
@@ -2020,13 +2020,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B67" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C67" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D67" t="s">
         <v>48</v>
@@ -2037,13 +2037,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B68" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D68" t="s">
         <v>5</v>
@@ -2054,13 +2054,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B69" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C69" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
         <v>49</v>
@@ -2071,13 +2071,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D70" t="s">
         <v>48</v>
@@ -2088,16 +2088,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E71" t="s">
         <v>55</v>
@@ -2105,13 +2105,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
       </c>
       <c r="C72" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D72" t="s">
         <v>48</v>
@@ -2122,13 +2122,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B73" t="s">
         <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D73" t="s">
         <v>5</v>
@@ -2139,13 +2139,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B74" t="s">
         <v>60</v>
       </c>
       <c r="C74" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D74" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Added More Generic Cards, Updated plugininfo.txt
</commit_message>
<xml_diff>
--- a/sets/carddata.xlsx
+++ b/sets/carddata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="176">
   <si>
     <t>Name</t>
   </si>
@@ -513,9 +513,6 @@
     <t>S220</t>
   </si>
   <si>
-    <t>Look Into the Future</t>
-  </si>
-  <si>
     <t>S221</t>
   </si>
   <si>
@@ -532,6 +529,33 @@
   </si>
   <si>
     <t>Flying Snake</t>
+  </si>
+  <si>
+    <t>Foresight</t>
+  </si>
+  <si>
+    <t>S223</t>
+  </si>
+  <si>
+    <t>S224</t>
+  </si>
+  <si>
+    <t>S225</t>
+  </si>
+  <si>
+    <t>S226</t>
+  </si>
+  <si>
+    <t>Chaos Wolf</t>
+  </si>
+  <si>
+    <t>Flaming Eagle</t>
+  </si>
+  <si>
+    <t>Ruins of the Night</t>
+  </si>
+  <si>
+    <t>Shrine of Everlasting Day</t>
   </si>
 </sst>
 </file>
@@ -883,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,7 +1381,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
@@ -1408,7 +1432,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>
@@ -2105,7 +2129,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
@@ -2122,13 +2146,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73" t="s">
         <v>60</v>
       </c>
       <c r="C73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D73" t="s">
         <v>5</v>
@@ -2139,19 +2163,87 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
         <v>60</v>
       </c>
       <c r="C74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D74" t="s">
         <v>48</v>
       </c>
       <c r="E74" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>172</v>
+      </c>
+      <c r="B75" t="s">
+        <v>60</v>
+      </c>
+      <c r="C75" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>173</v>
+      </c>
+      <c r="B76" t="s">
+        <v>60</v>
+      </c>
+      <c r="C76" t="s">
+        <v>169</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>174</v>
+      </c>
+      <c r="B77" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77" t="s">
+        <v>170</v>
+      </c>
+      <c r="D77" t="s">
+        <v>47</v>
+      </c>
+      <c r="E77" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>175</v>
+      </c>
+      <c r="B78" t="s">
+        <v>60</v>
+      </c>
+      <c r="C78" t="s">
+        <v>171</v>
+      </c>
+      <c r="D78" t="s">
+        <v>47</v>
+      </c>
+      <c r="E78" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Dragon and Dream Cards
Apparently Dragon's weren't in the last push, so they are now. Added Dream Kingdom.
</commit_message>
<xml_diff>
--- a/sets/carddata.xlsx
+++ b/sets/carddata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="207">
   <si>
     <t>Name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Structure</t>
   </si>
   <si>
-    <t>Magic</t>
-  </si>
-  <si>
     <t>Base</t>
   </si>
   <si>
@@ -516,9 +513,6 @@
     <t>S221</t>
   </si>
   <si>
-    <t>Ice Mammoth</t>
-  </si>
-  <si>
     <t>S222</t>
   </si>
   <si>
@@ -556,6 +550,105 @@
   </si>
   <si>
     <t>Shrine of Everlasting Day</t>
+  </si>
+  <si>
+    <t>S301</t>
+  </si>
+  <si>
+    <t>S302</t>
+  </si>
+  <si>
+    <t>S303</t>
+  </si>
+  <si>
+    <t>S304</t>
+  </si>
+  <si>
+    <t>S305</t>
+  </si>
+  <si>
+    <t>S306</t>
+  </si>
+  <si>
+    <t>S307</t>
+  </si>
+  <si>
+    <t>S308</t>
+  </si>
+  <si>
+    <t>S309</t>
+  </si>
+  <si>
+    <t>S310</t>
+  </si>
+  <si>
+    <t>S311</t>
+  </si>
+  <si>
+    <t>S312</t>
+  </si>
+  <si>
+    <t>S313</t>
+  </si>
+  <si>
+    <t>S314</t>
+  </si>
+  <si>
+    <t>Bergo, the Gifted</t>
+  </si>
+  <si>
+    <t>Dragon's Call</t>
+  </si>
+  <si>
+    <t>Dragon's Nest</t>
+  </si>
+  <si>
+    <t>The Dragon's Roar</t>
+  </si>
+  <si>
+    <t>Fire Breath</t>
+  </si>
+  <si>
+    <t>Fire Ball</t>
+  </si>
+  <si>
+    <t>Ice Breath</t>
+  </si>
+  <si>
+    <t>Kandreoth, Elemental Dragon</t>
+  </si>
+  <si>
+    <t>Kerdek, the Voiceless</t>
+  </si>
+  <si>
+    <t>Korgonterth, Deathlord</t>
+  </si>
+  <si>
+    <t>Lightning Breath</t>
+  </si>
+  <si>
+    <t>Poision Breath</t>
+  </si>
+  <si>
+    <t>Serg, Dragon Rider</t>
+  </si>
+  <si>
+    <t>Zanelle, Dragon Rider</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Spell</t>
+  </si>
+  <si>
+    <t>Dragon's World</t>
+  </si>
+  <si>
+    <t>S315</t>
+  </si>
+  <si>
+    <t>Elephant Statue</t>
   </si>
 </sst>
 </file>
@@ -899,7 +992,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -907,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -934,24 +1027,24 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -962,13 +1055,13 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -979,30 +1072,30 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" t="s">
         <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1013,30 +1106,30 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1047,30 +1140,30 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" t="s">
         <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1081,13 +1174,13 @@
         <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1098,13 +1191,13 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" t="s">
         <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1115,13 +1208,13 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1132,13 +1225,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1149,13 +1242,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1166,13 +1259,13 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
         <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1183,13 +1276,13 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1200,13 +1293,13 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1217,13 +1310,13 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1234,13 +1327,13 @@
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1251,13 +1344,13 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1268,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1285,30 +1378,30 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1319,13 +1412,13 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1336,13 +1429,13 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1353,13 +1446,13 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1370,30 +1463,30 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1404,13 +1497,13 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1421,47 +1514,47 @@
         <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
         <v>59</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
         <v>60</v>
       </c>
-      <c r="C32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" t="s">
-        <v>61</v>
-      </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1472,30 +1565,30 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" t="s">
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1506,13 +1599,13 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
       <c r="E35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1523,13 +1616,13 @@
         <v>42</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1540,13 +1633,13 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1557,13 +1650,13 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,13 +1667,13 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D39" t="s">
         <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1591,13 +1684,13 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1608,13 +1701,13 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1625,47 +1718,47 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1676,13 +1769,13 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1693,13 +1786,13 @@
         <v>42</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1710,13 +1803,13 @@
         <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1727,13 +1820,13 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1744,13 +1837,13 @@
         <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D49" t="s">
         <v>5</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1761,13 +1854,13 @@
         <v>42</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D50" t="s">
         <v>5</v>
       </c>
       <c r="E50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1778,13 +1871,13 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D51" t="s">
         <v>47</v>
       </c>
       <c r="E51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,454 +1888,709 @@
         <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D52" t="s">
         <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B53" t="s">
         <v>116</v>
       </c>
-      <c r="B53" t="s">
-        <v>117</v>
-      </c>
       <c r="C53" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D55" t="s">
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C56" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
       </c>
       <c r="E56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D57" t="s">
         <v>5</v>
       </c>
       <c r="E57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" t="s">
+        <v>116</v>
+      </c>
+      <c r="C58" t="s">
         <v>122</v>
       </c>
-      <c r="B58" t="s">
-        <v>117</v>
-      </c>
-      <c r="C58" t="s">
-        <v>123</v>
-      </c>
       <c r="D58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>128</v>
+      </c>
+      <c r="B59" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" t="s">
         <v>129</v>
       </c>
-      <c r="B59" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" t="s">
-        <v>130</v>
-      </c>
       <c r="D59" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>130</v>
+      </c>
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
         <v>131</v>
       </c>
-      <c r="B60" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" t="s">
-        <v>132</v>
-      </c>
       <c r="D60" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E60" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" t="s">
         <v>134</v>
       </c>
-      <c r="B61" t="s">
-        <v>117</v>
-      </c>
-      <c r="C61" t="s">
-        <v>135</v>
-      </c>
       <c r="D61" t="s">
         <v>5</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" t="s">
         <v>136</v>
       </c>
-      <c r="B62" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" t="s">
-        <v>137</v>
-      </c>
       <c r="D62" t="s">
         <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>137</v>
+      </c>
+      <c r="B63" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" t="s">
         <v>138</v>
       </c>
-      <c r="B63" t="s">
-        <v>117</v>
-      </c>
-      <c r="C63" t="s">
-        <v>139</v>
-      </c>
       <c r="D63" t="s">
         <v>5</v>
       </c>
       <c r="E63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" t="s">
         <v>140</v>
       </c>
-      <c r="B64" t="s">
-        <v>117</v>
-      </c>
-      <c r="C64" t="s">
-        <v>141</v>
-      </c>
       <c r="D64" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" t="s">
         <v>142</v>
       </c>
-      <c r="B65" t="s">
-        <v>117</v>
-      </c>
-      <c r="C65" t="s">
-        <v>143</v>
-      </c>
       <c r="D65" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" t="s">
         <v>144</v>
       </c>
-      <c r="B66" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" t="s">
-        <v>145</v>
-      </c>
       <c r="D66" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" t="s">
         <v>146</v>
       </c>
-      <c r="B67" t="s">
-        <v>117</v>
-      </c>
-      <c r="C67" t="s">
-        <v>147</v>
-      </c>
       <c r="D67" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" t="s">
         <v>148</v>
       </c>
-      <c r="B68" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68" t="s">
-        <v>149</v>
-      </c>
       <c r="D68" t="s">
         <v>5</v>
       </c>
       <c r="E68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" t="s">
         <v>150</v>
       </c>
-      <c r="B69" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" t="s">
-        <v>151</v>
-      </c>
       <c r="D69" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E69" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" t="s">
         <v>152</v>
       </c>
-      <c r="B70" t="s">
-        <v>117</v>
-      </c>
-      <c r="C70" t="s">
-        <v>153</v>
-      </c>
       <c r="D70" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" t="s">
         <v>154</v>
       </c>
-      <c r="B71" t="s">
-        <v>117</v>
-      </c>
-      <c r="C71" t="s">
-        <v>155</v>
-      </c>
       <c r="D71" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D72" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>162</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D73" t="s">
         <v>5</v>
       </c>
       <c r="E73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B74" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D74" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="E74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B75" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D75" t="s">
         <v>5</v>
       </c>
       <c r="E75" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D76" t="s">
         <v>5</v>
       </c>
       <c r="E76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B77" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C77" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D77" t="s">
         <v>47</v>
       </c>
       <c r="E77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D78" t="s">
         <v>47</v>
       </c>
       <c r="E78" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>188</v>
+      </c>
+      <c r="B79" t="s">
+        <v>202</v>
+      </c>
+      <c r="C79" t="s">
+        <v>174</v>
+      </c>
+      <c r="D79" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>189</v>
+      </c>
+      <c r="B80" t="s">
+        <v>202</v>
+      </c>
+      <c r="C80" t="s">
+        <v>175</v>
+      </c>
+      <c r="D80" t="s">
+        <v>203</v>
+      </c>
+      <c r="E80" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>190</v>
+      </c>
+      <c r="B81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C81" t="s">
+        <v>176</v>
+      </c>
+      <c r="D81" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>191</v>
+      </c>
+      <c r="B82" t="s">
+        <v>202</v>
+      </c>
+      <c r="C82" t="s">
+        <v>177</v>
+      </c>
+      <c r="D82" t="s">
+        <v>203</v>
+      </c>
+      <c r="E82" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>192</v>
+      </c>
+      <c r="B83" t="s">
+        <v>202</v>
+      </c>
+      <c r="C83" t="s">
+        <v>178</v>
+      </c>
+      <c r="D83" t="s">
+        <v>203</v>
+      </c>
+      <c r="E83" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+      <c r="B84" t="s">
+        <v>202</v>
+      </c>
+      <c r="C84" t="s">
+        <v>179</v>
+      </c>
+      <c r="D84" t="s">
+        <v>203</v>
+      </c>
+      <c r="E84" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>194</v>
+      </c>
+      <c r="B85" t="s">
+        <v>202</v>
+      </c>
+      <c r="C85" t="s">
+        <v>180</v>
+      </c>
+      <c r="D85" t="s">
+        <v>203</v>
+      </c>
+      <c r="E85" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>195</v>
+      </c>
+      <c r="B86" t="s">
+        <v>202</v>
+      </c>
+      <c r="C86" t="s">
+        <v>181</v>
+      </c>
+      <c r="D86" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>196</v>
+      </c>
+      <c r="B87" t="s">
+        <v>202</v>
+      </c>
+      <c r="C87" t="s">
+        <v>182</v>
+      </c>
+      <c r="D87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>197</v>
+      </c>
+      <c r="B88" t="s">
+        <v>202</v>
+      </c>
+      <c r="C88" t="s">
+        <v>183</v>
+      </c>
+      <c r="D88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>198</v>
+      </c>
+      <c r="B89" t="s">
+        <v>202</v>
+      </c>
+      <c r="C89" t="s">
+        <v>184</v>
+      </c>
+      <c r="D89" t="s">
+        <v>203</v>
+      </c>
+      <c r="E89" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>199</v>
+      </c>
+      <c r="B90" t="s">
+        <v>202</v>
+      </c>
+      <c r="C90" t="s">
+        <v>185</v>
+      </c>
+      <c r="D90" t="s">
+        <v>203</v>
+      </c>
+      <c r="E90" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>200</v>
+      </c>
+      <c r="B91" t="s">
+        <v>202</v>
+      </c>
+      <c r="C91" t="s">
+        <v>186</v>
+      </c>
+      <c r="D91" t="s">
+        <v>5</v>
+      </c>
+      <c r="E91" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>201</v>
+      </c>
+      <c r="B92" t="s">
+        <v>202</v>
+      </c>
+      <c r="C92" t="s">
+        <v>187</v>
+      </c>
+      <c r="D92" t="s">
+        <v>5</v>
+      </c>
+      <c r="E92" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>204</v>
+      </c>
+      <c r="B93" t="s">
+        <v>202</v>
+      </c>
+      <c r="C93" t="s">
+        <v>205</v>
+      </c>
+      <c r="D93" t="s">
+        <v>48</v>
+      </c>
+      <c r="E93" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Dragons and Dreams
Dragons and Dreams stopped working, fixed by saving the tabe delimited text file again.
</commit_message>
<xml_diff>
--- a/sets/carddata.xlsx
+++ b/sets/carddata.xlsx
@@ -1061,7 +1061,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>